<commit_message>
revision de solicitud y aprobacion de peticion
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Cambios/Solicitud_Cambios-150615.xlsx
+++ b/qualtcom/Procesos/Cambios/Solicitud_Cambios-150615.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Datos Generales</t>
   </si>
@@ -280,6 +280,18 @@
   </si>
   <si>
     <t>1 hr</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>Fidel Reyna</t>
+  </si>
+  <si>
+    <t>44.62</t>
+  </si>
+  <si>
+    <t>No aplica</t>
   </si>
 </sst>
 </file>
@@ -950,6 +962,9 @@
     <xf numFmtId="0" fontId="26" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -964,9 +979,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="87">
@@ -1621,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1908,7 +1920,7 @@
       <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -1924,7 +1936,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="26"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
@@ -1939,21 +1951,21 @@
       <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="26"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="25"/>
       <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="26"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="13" t="s">
@@ -1965,7 +1977,7 @@
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
@@ -2001,10 +2013,10 @@
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="24"/>
+      <c r="C11" s="25"/>
       <c r="E11" s="9"/>
       <c r="F11" s="4"/>
     </row>
@@ -2028,7 +2040,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="23" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -2039,7 +2051,9 @@
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
+      <c r="G13" s="14">
+        <v>42171</v>
+      </c>
       <c r="H13" s="13" t="s">
         <v>44</v>
       </c>
@@ -2221,79 +2235,97 @@
     </row>
     <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="27"/>
+      <c r="C34" s="28"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
       <c r="B35" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
       <c r="B36" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
       <c r="B37" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="13"/>
+      <c r="C37" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
       <c r="B38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13"/>
+      <c r="C38" s="14">
+        <v>42171</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="13"/>
+      <c r="C39" s="14">
+        <v>42171</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="C40" s="14">
+        <v>42171</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="23"/>
+      <c r="C41" s="24"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
       <c r="B42" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="13"/>
+      <c r="C42" s="13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="13"/>
+      <c r="C43" s="14">
+        <v>42171</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B44" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="13"/>
+      <c r="C44" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2325,15 +2357,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Listo para revisión</Status>
@@ -2346,6 +2369,15 @@
     </Owner>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2433,14 +2465,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{862920E9-66EB-4C3E-957A-EA8E4211520C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2451,6 +2475,14 @@
     <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Aprobacion de cambio documento cambios por impresora
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Cambios/Solicitud_Cambios-150615.xlsx
+++ b/qualtcom/Procesos/Cambios/Solicitud_Cambios-150615.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Cambios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Procesos\Cambios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1633,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1943,7 +1943,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -2357,6 +2357,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Listo para revisión</Status>
@@ -2369,15 +2378,6 @@
     </Owner>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2465,6 +2465,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{862920E9-66EB-4C3E-957A-EA8E4211520C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2475,14 +2483,6 @@
     <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>